<commit_message>
fix: bonus penghasilan lainnya
</commit_message>
<xml_diff>
--- a/public/template_penghasilan_lainnya.xlsx
+++ b/public/template_penghasilan_lainnya.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\kerja\hcs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2039CDF-1E57-413B-BD5C-E13124A1AEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754004E-42FC-4D4A-B177-AC6FFE3C9AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C44F0C1-B7AA-4D81-8DCC-17FF49DA3032}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>nip</t>
-  </si>
-  <si>
-    <t>kategori</t>
   </si>
   <si>
     <t>nominal</t>
@@ -78,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,26 +392,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E33FEA-C6AA-4137-B3C4-C542D873D9F9}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: list penghasilan teratur
</commit_message>
<xml_diff>
--- a/public/template_penghasilan_lainnya.xlsx
+++ b/public/template_penghasilan_lainnya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\kerja\hcs\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F754004E-42FC-4D4A-B177-AC6FFE3C9AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0816485E-DE5C-4306-B6BE-4A2CA1F9FFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9C44F0C1-B7AA-4D81-8DCC-17FF49DA3032}"/>
   </bookViews>
@@ -34,19 +34,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>nip</t>
   </si>
   <si>
     <t>nominal</t>
   </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>00124</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +60,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,15 +89,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E33FEA-C6AA-4137-B3C4-C542D873D9F9}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,11 +441,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>